<commit_message>
Repository tidying up Sept 2024
</commit_message>
<xml_diff>
--- a/Data/IPWP_ExtractedAnomalies.xlsx
+++ b/Data/IPWP_ExtractedAnomalies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob.sharepoint.com/teams/grp-Chapter4-Leo/Shared Documents/General/Results/HadlSST/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardobertini/PycharmProjects/PoritesGrowthBaselines/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{402EA9D0-E1D8-2345-BAA4-D5E026A6B115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{569A98F2-880E-0E4A-8737-C2E22A0334FD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B44C660-572D-9C48-BAEA-6B2E144A6B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1220" windowWidth="27640" windowHeight="16760" xr2:uid="{C4EDA56D-9F7A-3C45-A4E3-C2FC382C59F9}"/>
   </bookViews>
@@ -117,14 +117,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>447419</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>325119</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>72729</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>370745</xdr:colOff>
+      <xdr:colOff>370744</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>53679</xdr:rowOff>
     </xdr:to>
@@ -143,13 +143,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect r="37271"/>
+        <a:srcRect l="9041" r="37272"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5693071" y="72729"/>
-          <a:ext cx="4892892" cy="4903186"/>
+          <a:off x="6990079" y="72729"/>
+          <a:ext cx="4160425" cy="4857750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E4235E-4296-764C-97DB-7AE9B35D56A8}">
   <dimension ref="A1:F379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,7 +513,7 @@
         <v>1781.6816143497699</v>
       </c>
       <c r="B2" s="1">
-        <f t="shared" ref="B2:B33" si="0">ROUND(A2,0)</f>
+        <f>ROUND(A2,0)</f>
         <v>1782</v>
       </c>
       <c r="C2" s="1">
@@ -524,7 +524,7 @@
         <v>1782</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F33" si="1">AVERAGEIF($B$2:$B$378,B2,$C$2:$C$378)</f>
+        <f>AVERAGEIF($B$2:$B$378,B2,$C$2:$C$378)</f>
         <v>-0.46118949391415698</v>
       </c>
     </row>
@@ -533,7 +533,7 @@
         <v>1782.59985399937</v>
       </c>
       <c r="B3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B2:B33" si="0">ROUND(A3,0)</f>
         <v>1783</v>
       </c>
       <c r="C3">
@@ -543,7 +543,7 @@
         <v>1783</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F2:F33" si="1">AVERAGEIF($B$2:$B$378,B3,$C$2:$C$378)</f>
         <v>-0.12907008327994801</v>
       </c>
     </row>
@@ -1877,15 +1877,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004253EC1B5825C440A773F29DC75B7BF8" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7ed15c621f4faaa91353e3056749fe29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="54f3b4ec-13a1-4634-8b82-ecc475231c60" xmlns:ns3="e9f2c45d-f6b2-408e-a590-c46263d37de1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a31c0a8274f8dc19dc14c3a10ef4344" ns2:_="" ns3:_="">
     <xsd:import namespace="54f3b4ec-13a1-4634-8b82-ecc475231c60"/>
@@ -2108,15 +2099,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C12F30C-5850-4103-8399-CEE08D05DC55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DCA9352-0FDF-431D-9A7A-15B6AF19606A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2133,4 +2125,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C12F30C-5850-4103-8399-CEE08D05DC55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>